<commit_message>
keywords list modifed to include keywords for news parsing
</commit_message>
<xml_diff>
--- a/src/templates/keywords.xlsx
+++ b/src/templates/keywords.xlsx
@@ -6,6 +6,7 @@
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист1" sheetId="3" r:id="rId3"/>
+    <sheet name="news_keywords" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -665,4 +666,48 @@
     <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>keyword</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>News</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>news</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>новости</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>novosti</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>novosty</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A6"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>